<commit_message>
ReadMe Edit & Added Dataset
Updated the ReadMe with links to datasets and added information on cloud cover's affect on solar panel proficiency. Also added a question about carbon offset.

Added datasets for energy production by state.
</commit_message>
<xml_diff>
--- a/Chart To Do List.xlsx
+++ b/Chart To Do List.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Data Viz Projects\The_Dirty_Hippy_Proposal_For_Clean_Solar_Energy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA46870-8EE6-4E1C-A2E9-353FF4A96CE2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0238ED16-D826-4B43-9A14-DF8E56CF1C32}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{06FDBFB9-0260-41AD-8906-A49EB2D83A74}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{06FDBFB9-0260-41AD-8906-A49EB2D83A74}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Charts to Make" sheetId="1" r:id="rId1"/>
+    <sheet name="Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="39">
   <si>
     <t>Chart To-Do List</t>
   </si>
@@ -115,6 +116,39 @@
   </si>
   <si>
     <t>Completed?3</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Bar Chart</t>
+  </si>
+  <si>
+    <t>Scatter Plot</t>
+  </si>
+  <si>
+    <t>Name of the State</t>
+  </si>
+  <si>
+    <t>Landmass of the state, no large bodies of water</t>
+  </si>
+  <si>
+    <t>Population of the State</t>
+  </si>
+  <si>
+    <t>State Population divided by State Landmass</t>
+  </si>
+  <si>
+    <t>Total carbon offset according to Google's Project Sunroof</t>
+  </si>
+  <si>
+    <t>Total Carbon Offset adjusted for percent of sunlight by state and percent of clean energy produced by state</t>
+  </si>
+  <si>
+    <t>Not actually a heat map, but I'm not sure of the actaul name. Will be a map with colored values</t>
   </si>
 </sst>
 </file>
@@ -402,7 +436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -434,6 +468,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -446,33 +489,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -652,6 +676,12 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
@@ -659,15 +689,22 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <left style="medium">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="medium">
+        <right style="thin">
           <color indexed="64"/>
         </right>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
   </dxfs>
@@ -684,21 +721,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{901C8E68-FC53-4A98-9367-6100525EF00C}" name="Table5" displayName="Table5" ref="B4:J14" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="10" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{901C8E68-FC53-4A98-9367-6100525EF00C}" name="Table5" displayName="Table5" ref="B4:J14" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
   <autoFilter ref="B4:J14" xr:uid="{C7C9638A-BB53-4224-B46B-A88831222D9E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B5:J14">
     <sortCondition ref="B4:B14"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{E621C5C3-0F6B-4E04-8273-4CD5F8D471A7}" name="Number" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{B364F0ED-253B-40A5-B1B6-7883E75E0691}" name="Chart Title" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{F336DDEC-DB6B-43C6-A3B9-17C04E3300D1}" name="Type" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{0383B459-17EB-4659-8FD5-E5AEB1C659C6}" name="Completed?" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{E7E5E3FD-F032-4ECC-A592-3078E862C7CF}" name="X-Axis title" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{365F08F1-80FF-479B-A296-C70415CBC490}" name="Completed?2" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{323F3600-1A85-43DB-AA62-DAC1738EBE17}" name="Y-Axis Title" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{ABD08D9C-389E-41D5-B9AF-037818EF5DF3}" name="Completed?3" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{CD3D8F98-660B-49CC-9DEC-DFB232B34E99}" name="Notes" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{E621C5C3-0F6B-4E04-8273-4CD5F8D471A7}" name="Number" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{B364F0ED-253B-40A5-B1B6-7883E75E0691}" name="Chart Title" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{F336DDEC-DB6B-43C6-A3B9-17C04E3300D1}" name="Type" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{0383B459-17EB-4659-8FD5-E5AEB1C659C6}" name="Completed?" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{E7E5E3FD-F032-4ECC-A592-3078E862C7CF}" name="X-Axis title" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{365F08F1-80FF-479B-A296-C70415CBC490}" name="Completed?2" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{323F3600-1A85-43DB-AA62-DAC1738EBE17}" name="Y-Axis Title" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{ABD08D9C-389E-41D5-B9AF-037818EF5DF3}" name="Completed?3" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{CD3D8F98-660B-49CC-9DEC-DFB232B34E99}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1004,7 +1041,7 @@
   <dimension ref="B1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,31 +1059,31 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="19"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="22"/>
     </row>
     <row r="3" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="23" t="s">
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="19"/>
       <c r="J3" s="15"/>
     </row>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1360,4 +1397,103 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0754CEB-EFE7-43D6-BC2B-AF53D77D9D66}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added & Edited Datasets
Found a new dataset for State Landmass. It needs a lot of cleaning. Changed the dataset of state abbreviations so that it showed state names as well.
</commit_message>
<xml_diff>
--- a/Chart To Do List.xlsx
+++ b/Chart To Do List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Data Viz Projects\The_Dirty_Hippy_Proposal_For_Clean_Solar_Energy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Grattendick\Desktop\The_Dirty_Hippy_Proposal_For_Clean_Solar_Energy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0238ED16-D826-4B43-9A14-DF8E56CF1C32}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DFFDE6-840E-4371-9683-778C0175388B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{06FDBFB9-0260-41AD-8906-A49EB2D83A74}"/>
+    <workbookView xWindow="21480" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{06FDBFB9-0260-41AD-8906-A49EB2D83A74}"/>
   </bookViews>
   <sheets>
     <sheet name="Charts to Make" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="40">
   <si>
     <t>Chart To-Do List</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>Not actually a heat map, but I'm not sure of the actaul name. Will be a map with colored values</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -178,7 +181,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,6 +194,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -436,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -468,6 +477,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -489,9 +501,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1041,7 +1052,7 @@
   <dimension ref="B1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1059,31 +1070,31 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="23"/>
     </row>
     <row r="3" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="17" t="s">
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="20"/>
       <c r="J3" s="15"/>
     </row>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1131,8 +1142,8 @@
       <c r="F5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>19</v>
+      <c r="G5" s="25" t="s">
+        <v>39</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>20</v>
@@ -1158,8 +1169,8 @@
       <c r="F6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>19</v>
+      <c r="G6" s="26" t="s">
+        <v>39</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>21</v>
@@ -1185,8 +1196,8 @@
       <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>19</v>
+      <c r="G7" s="26" t="s">
+        <v>39</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>21</v>
@@ -1441,7 +1452,7 @@
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="17" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1489,7 +1500,7 @@
       <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="17" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added & Edited Datasets, Edited ReadMe
Found and added datasets for state landmass and populations. Edited ReadMe to reflect this new information and their sources.
</commit_message>
<xml_diff>
--- a/Chart To Do List.xlsx
+++ b/Chart To Do List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Grattendick\Desktop\The_Dirty_Hippy_Proposal_For_Clean_Solar_Energy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DFFDE6-840E-4371-9683-778C0175388B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C28881-79B3-44DD-8D16-FA7D6C318C73}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21480" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{06FDBFB9-0260-41AD-8906-A49EB2D83A74}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="40">
   <si>
     <t>Chart To-Do List</t>
   </si>
@@ -480,6 +480,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -501,8 +503,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1052,7 +1052,7 @@
   <dimension ref="B1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,31 +1070,31 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="25"/>
     </row>
     <row r="3" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="18" t="s">
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="20"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="22"/>
       <c r="J3" s="15"/>
     </row>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1142,7 +1142,7 @@
       <c r="F5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="25" t="s">
+      <c r="G5" s="18" t="s">
         <v>39</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -1169,7 +1169,7 @@
       <c r="F6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="19" t="s">
         <v>39</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -1196,7 +1196,7 @@
       <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="19" t="s">
         <v>39</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -1223,8 +1223,8 @@
       <c r="F8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>19</v>
+      <c r="G8" s="19" t="s">
+        <v>39</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>21</v>
@@ -1250,8 +1250,8 @@
       <c r="F9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>19</v>
+      <c r="G9" s="19" t="s">
+        <v>39</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>21</v>
@@ -1277,8 +1277,8 @@
       <c r="F10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>19</v>
+      <c r="G10" s="19" t="s">
+        <v>39</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>21</v>
@@ -1304,8 +1304,8 @@
       <c r="F11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>19</v>
+      <c r="G11" s="19" t="s">
+        <v>39</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>21</v>
@@ -1331,8 +1331,8 @@
       <c r="F12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>19</v>
+      <c r="G12" s="19" t="s">
+        <v>39</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>21</v>
@@ -1415,7 +1415,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Data Munging & Plot Work
Cleaned up the Project Sunroof State CSV to just have U.S. states. Started plotting the total carbon offset by state bar plot with pandas.
</commit_message>
<xml_diff>
--- a/Chart To Do List.xlsx
+++ b/Chart To Do List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Grattendick\Desktop\The_Dirty_Hippy_Proposal_For_Clean_Solar_Energy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B06852C-24DB-4E77-B895-F374F89B6B39}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1650B560-4093-4B49-A0B0-D5764A275923}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21480" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{06FDBFB9-0260-41AD-8906-A49EB2D83A74}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="42">
   <si>
     <t>Chart To-Do List</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>Yed</t>
+  </si>
+  <si>
+    <t>In Progress</t>
   </si>
 </sst>
 </file>
@@ -184,7 +187,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,6 +206,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="19">
     <border>
@@ -453,7 +462,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -485,6 +493,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -506,7 +515,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1056,7 +1065,7 @@
   <dimension ref="B1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1099,39 +1108,39 @@
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
       <c r="I3" s="22"/>
-      <c r="J3" s="15"/>
+      <c r="J3" s="14"/>
     </row>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1140,25 +1149,25 @@
       <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>19</v>
+      <c r="E5" s="27" t="s">
+        <v>41</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="17" t="s">
         <v>39</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="9"/>
+      <c r="I5" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="8"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -1173,7 +1182,7 @@
       <c r="F6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="19" t="s">
+      <c r="G6" s="18" t="s">
         <v>39</v>
       </c>
       <c r="H6" s="1" t="s">
@@ -1182,10 +1191,10 @@
       <c r="I6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="10"/>
+      <c r="J6" s="9"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -1200,7 +1209,7 @@
       <c r="F7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="18" t="s">
         <v>39</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -1209,10 +1218,10 @@
       <c r="I7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="10"/>
+      <c r="J7" s="9"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>4</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1227,7 +1236,7 @@
       <c r="F8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="19" t="s">
+      <c r="G8" s="18" t="s">
         <v>39</v>
       </c>
       <c r="H8" s="1" t="s">
@@ -1236,10 +1245,10 @@
       <c r="I8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="10"/>
+      <c r="J8" s="9"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>5</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1254,7 +1263,7 @@
       <c r="F9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="18" t="s">
         <v>39</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -1263,10 +1272,10 @@
       <c r="I9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="10"/>
+      <c r="J9" s="9"/>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>6</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1281,7 +1290,7 @@
       <c r="F10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="18" t="s">
         <v>39</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -1290,10 +1299,10 @@
       <c r="I10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="10"/>
+      <c r="J10" s="9"/>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="7">
+      <c r="B11" s="6">
         <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1308,7 +1317,7 @@
       <c r="F11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="18" t="s">
         <v>39</v>
       </c>
       <c r="H11" s="1" t="s">
@@ -1317,10 +1326,10 @@
       <c r="I11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J11" s="10"/>
+      <c r="J11" s="9"/>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>8</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -1335,7 +1344,7 @@
       <c r="F12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="18" t="s">
         <v>39</v>
       </c>
       <c r="H12" s="1" t="s">
@@ -1344,10 +1353,10 @@
       <c r="I12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="10"/>
+      <c r="J12" s="9"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1362,7 +1371,7 @@
       <c r="F13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="18" t="s">
         <v>40</v>
       </c>
       <c r="H13" s="1" t="s">
@@ -1371,34 +1380,34 @@
       <c r="I13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="10"/>
+      <c r="J13" s="9"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="11">
+      <c r="B14" s="10">
         <v>10</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="12" t="s">
+      <c r="E14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="27" t="s">
+      <c r="G14" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="H14" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="J14" s="14"/>
+      <c r="I14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1419,7 +1428,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,7 +1465,7 @@
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1504,7 +1513,7 @@
       <c r="A10" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Data Statistics & Plot Work
Calculated the adjusted carbon offset from the total carbon offset. Started plotting adjusted carbon offset by state.
</commit_message>
<xml_diff>
--- a/Chart To Do List.xlsx
+++ b/Chart To Do List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Grattendick\Desktop\The_Dirty_Hippy_Proposal_For_Clean_Solar_Energy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D87DEDF-7864-4E96-A4E4-82856F9C4985}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DEA05C-85BD-4556-B835-02BDC73F2CBD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21480" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{06FDBFB9-0260-41AD-8906-A49EB2D83A74}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="42">
   <si>
     <t>Chart To-Do List</t>
   </si>
@@ -494,6 +494,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -515,7 +516,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1065,7 +1065,7 @@
   <dimension ref="B1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,31 +1083,31 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="26"/>
     </row>
     <row r="3" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="20" t="s">
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="23"/>
       <c r="J3" s="14"/>
     </row>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1176,8 +1176,8 @@
       <c r="D6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>19</v>
+      <c r="E6" s="20" t="s">
+        <v>41</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>22</v>
@@ -1188,8 +1188,8 @@
       <c r="H6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="27" t="s">
-        <v>41</v>
+      <c r="I6" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="J6" s="9"/>
     </row>
@@ -1215,8 +1215,8 @@
       <c r="H7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="27" t="s">
-        <v>41</v>
+      <c r="I7" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="J7" s="9"/>
     </row>
@@ -1242,8 +1242,8 @@
       <c r="H8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="27" t="s">
-        <v>41</v>
+      <c r="I8" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="J8" s="9"/>
     </row>
@@ -1269,8 +1269,8 @@
       <c r="H9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I9" s="27" t="s">
-        <v>41</v>
+      <c r="I9" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="J9" s="9"/>
     </row>
@@ -1296,8 +1296,8 @@
       <c r="H10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="27" t="s">
-        <v>41</v>
+      <c r="I10" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="J10" s="9"/>
     </row>
@@ -1323,8 +1323,8 @@
       <c r="H11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="27" t="s">
-        <v>41</v>
+      <c r="I11" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="J11" s="9"/>
     </row>
@@ -1350,8 +1350,8 @@
       <c r="H12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="27" t="s">
-        <v>41</v>
+      <c r="I12" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="J12" s="9"/>
     </row>
@@ -1377,8 +1377,8 @@
       <c r="H13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="27" t="s">
-        <v>41</v>
+      <c r="I13" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="J13" s="9"/>
     </row>
@@ -1404,8 +1404,8 @@
       <c r="H14" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="27" t="s">
-        <v>41</v>
+      <c r="I14" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="J14" s="13"/>
     </row>

</xml_diff>

<commit_message>
Plot Work & ReadMe Edit
Worked on state landmass scatter plot with the dropped states. Realized that state landmass might is not as useful as originally thought, and discussed that in the readme file.
</commit_message>
<xml_diff>
--- a/Chart To Do List.xlsx
+++ b/Chart To Do List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Grattendick\Desktop\The_Dirty_Hippy_Proposal_For_Clean_Solar_Energy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28B68BF-95ED-456C-BFE9-F4EE5FB83638}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F26F4DB-EC01-4D08-B001-23FFE6265CB2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{06FDBFB9-0260-41AD-8906-A49EB2D83A74}"/>
   </bookViews>
@@ -483,6 +483,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -504,7 +505,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1054,7 +1054,7 @@
   <dimension ref="B1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,31 +1073,31 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="25"/>
     </row>
     <row r="3" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="19" t="s">
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="22"/>
       <c r="J3" s="13"/>
     </row>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1249,7 +1249,7 @@
       <c r="D9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="19" t="s">
         <v>42</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -1303,8 +1303,8 @@
       <c r="D11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>19</v>
+      <c r="E11" s="19" t="s">
+        <v>42</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>23</v>

</xml_diff>